<commit_message>
Updated BOM and zip
</commit_message>
<xml_diff>
--- a/PiZeroAudioI2S-31-Oct-18.xlsx
+++ b/PiZeroAudioI2S-31-Oct-18.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angelofraietta/Documents/eagle/projects/HappyBracketsPiHats/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8BA29E76-AF43-B644-95AA-8AB7DAD3679E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="30680" yWindow="1980" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="30675" yWindow="1980" windowWidth="28035" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="PiZeroAudioI2S-31-Oct-18" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -82,9 +76,6 @@
     <t>C18, C35</t>
   </si>
   <si>
-    <t>Polarised capacitor 0603 Footprint</t>
-  </si>
-  <si>
     <t>TLJA107M010R1400</t>
   </si>
   <si>
@@ -412,17 +403,20 @@
     <t>TXS0102DCURG4</t>
   </si>
   <si>
-    <t>80K</t>
-  </si>
-  <si>
-    <t>PTN0603E8002BST1</t>
+    <t xml:space="preserve">Polarised capacitor </t>
+  </si>
+  <si>
+    <t>CRCW060376K8FKEA</t>
+  </si>
+  <si>
+    <t>76K8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1009,7 +1003,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1061,7 +1055,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1255,28 +1249,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="6" max="6" width="32.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="83" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1293,7 +1288,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1316,7 +1311,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>9</v>
       </c>
@@ -1324,7 +1319,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -1333,13 +1328,13 @@
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1347,7 +1342,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -1359,64 +1354,64 @@
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>24</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>25</v>
       </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" t="s">
-        <v>29</v>
-      </c>
       <c r="G7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
@@ -1425,21 +1420,21 @@
         <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
         <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -1448,21 +1443,21 @@
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -1471,21 +1466,21 @@
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1494,21 +1489,21 @@
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
@@ -1517,13 +1512,13 @@
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1531,30 +1526,30 @@
         <v>220</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
         <v>23</v>
       </c>
-      <c r="E13" t="s">
-        <v>24</v>
-      </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>4</v>
       </c>
       <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
         <v>43</v>
-      </c>
-      <c r="C14" t="s">
-        <v>44</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
@@ -1563,421 +1558,422 @@
         <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
         <v>45</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
         <v>46</v>
       </c>
-      <c r="D15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>47</v>
       </c>
-      <c r="G15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" t="s">
         <v>49</v>
       </c>
-      <c r="C16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>50</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>51</v>
       </c>
-      <c r="G16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" t="s">
         <v>53</v>
       </c>
-      <c r="C17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" t="s">
-        <v>54</v>
-      </c>
       <c r="G17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" t="s">
         <v>56</v>
       </c>
-      <c r="C18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" t="s">
-        <v>57</v>
-      </c>
       <c r="G18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>2</v>
       </c>
       <c r="B19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" t="s">
         <v>130</v>
       </c>
-      <c r="C19" t="s">
-        <v>131</v>
-      </c>
       <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" t="s">
         <v>23</v>
       </c>
-      <c r="E19" t="s">
-        <v>24</v>
-      </c>
       <c r="F19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
         <v>60</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" t="s">
         <v>61</v>
       </c>
-      <c r="D20" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" t="s">
         <v>63</v>
       </c>
-      <c r="C21" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" t="s">
-        <v>64</v>
-      </c>
       <c r="G21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" t="s">
         <v>66</v>
       </c>
-      <c r="C22" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>67</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>68</v>
       </c>
-      <c r="G22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>4</v>
       </c>
       <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
+        <v>124</v>
+      </c>
+      <c r="D23" t="s">
         <v>71</v>
       </c>
-      <c r="C23" t="s">
-        <v>125</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>72</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>73</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>74</v>
       </c>
-      <c r="G23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C24">
         <v>110990030</v>
       </c>
       <c r="D24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" t="s">
         <v>76</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>77</v>
       </c>
-      <c r="F24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>1</v>
       </c>
       <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" t="s">
         <v>79</v>
       </c>
-      <c r="C25" t="s">
-        <v>126</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>80</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>81</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>82</v>
       </c>
-      <c r="G25" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" t="s">
         <v>84</v>
       </c>
-      <c r="C26" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>85</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>86</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>87</v>
       </c>
-      <c r="G26" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" t="s">
         <v>90</v>
       </c>
-      <c r="C27" t="s">
-        <v>94</v>
-      </c>
-      <c r="D27" t="s">
-        <v>90</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>91</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>92</v>
       </c>
-      <c r="G27" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" t="s">
         <v>95</v>
       </c>
-      <c r="C28" t="s">
-        <v>127</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>96</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>97</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>98</v>
       </c>
-      <c r="G28" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" t="s">
+        <v>119</v>
+      </c>
+      <c r="F29" t="s">
         <v>100</v>
       </c>
-      <c r="C29" t="s">
-        <v>128</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="G29" t="s">
         <v>118</v>
       </c>
-      <c r="E29" t="s">
-        <v>120</v>
-      </c>
-      <c r="F29" t="s">
-        <v>101</v>
-      </c>
-      <c r="G29" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30" t="s">
         <v>102</v>
       </c>
-      <c r="C30" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" t="s">
-        <v>102</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>103</v>
       </c>
-      <c r="F30" t="s">
-        <v>104</v>
-      </c>
       <c r="G30" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" t="s">
         <v>105</v>
       </c>
-      <c r="C31" t="s">
-        <v>105</v>
-      </c>
-      <c r="D31" t="s">
-        <v>105</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>106</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>107</v>
       </c>
-      <c r="G31" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" t="s">
         <v>109</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D32" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>110</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>111</v>
-      </c>
-      <c r="G32" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>